<commit_message>
'update report 2nd round'
</commit_message>
<xml_diff>
--- a/dcd_top_offset_step_tsmc2p_meas.xlsx
+++ b/dcd_top_offset_step_tsmc2p_meas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5132" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5172" uniqueCount="323">
   <si>
     <t>Process</t>
   </si>
@@ -926,6 +926,9 @@
   </si>
   <si>
     <t>tsmc2p (192)</t>
+  </si>
+  <si>
+    <t>n/a</t>
   </si>
   <si>
     <t>tsmc2p (193)</t>
@@ -986,7 +989,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1009,8 +1012,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000 "/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1029,6 +1039,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1042,11 +1058,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1444,10 +1461,10 @@
         <v>29</v>
       </c>
       <c r="O2" s="2">
-        <v>49.9197</v>
+        <v>36.9052</v>
       </c>
       <c r="P2">
-        <v>6.65625</v>
+        <v>4.92096</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -1494,10 +1511,10 @@
         <v>29</v>
       </c>
       <c r="O3" s="2">
-        <v>48.5773</v>
+        <v>35.9754</v>
       </c>
       <c r="P3">
-        <v>6.47725</v>
+        <v>4.79699</v>
       </c>
     </row>
     <row r="4" spans="1:16">
@@ -1543,11 +1560,11 @@
       <c r="N4" t="s">
         <v>29</v>
       </c>
-      <c r="O4" s="2">
-        <v>46.6643</v>
+      <c r="O4">
+        <v>34.3209</v>
       </c>
       <c r="P4">
-        <v>6.22219</v>
+        <v>4.5764</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -1593,11 +1610,11 @@
       <c r="N5" t="s">
         <v>29</v>
       </c>
-      <c r="O5" s="2">
-        <v>45.3222</v>
+      <c r="O5">
+        <v>33.3392</v>
       </c>
       <c r="P5">
-        <v>6.04325</v>
+        <v>4.44552</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -1643,11 +1660,11 @@
       <c r="N6" t="s">
         <v>29</v>
       </c>
-      <c r="O6" s="2">
-        <v>44.8052</v>
+      <c r="O6">
+        <v>32.8749</v>
       </c>
       <c r="P6">
-        <v>5.97431</v>
+        <v>4.38361</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -1693,11 +1710,11 @@
       <c r="N7" t="s">
         <v>29</v>
       </c>
-      <c r="O7" s="2">
-        <v>43.5655</v>
+      <c r="O7">
+        <v>31.8935</v>
       </c>
       <c r="P7">
-        <v>5.80903</v>
+        <v>4.25964</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -1743,11 +1760,11 @@
       <c r="N8" t="s">
         <v>29</v>
       </c>
-      <c r="O8" s="2">
-        <v>42.4809</v>
+      <c r="O8">
+        <v>31.0163</v>
       </c>
       <c r="P8">
-        <v>5.66441</v>
+        <v>4.1358</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -1793,11 +1810,11 @@
       <c r="N9" t="s">
         <v>29</v>
       </c>
-      <c r="O9" s="2">
-        <v>41.3448</v>
+      <c r="O9">
+        <v>30.1895</v>
       </c>
       <c r="P9">
-        <v>5.51292</v>
+        <v>4.02556</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -1843,11 +1860,11 @@
       <c r="N10" t="s">
         <v>29</v>
       </c>
-      <c r="O10" s="2">
-        <v>42.2226</v>
+      <c r="O10">
+        <v>30.4475</v>
       </c>
       <c r="P10">
-        <v>5.62998</v>
+        <v>4.05995</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -1893,11 +1910,11 @@
       <c r="N11" t="s">
         <v>29</v>
       </c>
-      <c r="O11" s="2">
-        <v>41.1386</v>
+      <c r="O11">
+        <v>29.5181</v>
       </c>
       <c r="P11">
-        <v>5.48545</v>
+        <v>3.93604</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -1943,11 +1960,11 @@
       <c r="N12" t="s">
         <v>29</v>
       </c>
-      <c r="O12" s="2">
-        <v>40.0544</v>
+      <c r="O12">
+        <v>28.7435</v>
       </c>
       <c r="P12">
-        <v>5.34089</v>
+        <v>3.83275</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -1993,11 +2010,11 @@
       <c r="N13" t="s">
         <v>29</v>
       </c>
-      <c r="O13" s="2">
-        <v>38.918</v>
+      <c r="O13">
+        <v>27.814</v>
       </c>
       <c r="P13">
-        <v>5.18935</v>
+        <v>3.70884</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -2043,11 +2060,11 @@
       <c r="N14" t="s">
         <v>29</v>
       </c>
-      <c r="O14" s="2">
-        <v>38.4013</v>
+      <c r="O14">
+        <v>27.2459</v>
       </c>
       <c r="P14">
-        <v>5.12046</v>
+        <v>3.63307</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -2093,11 +2110,11 @@
       <c r="N15" t="s">
         <v>29</v>
       </c>
-      <c r="O15" s="2">
-        <v>37.2135</v>
+      <c r="O15">
+        <v>26.2663</v>
       </c>
       <c r="P15">
-        <v>4.96209</v>
+        <v>3.50245</v>
       </c>
     </row>
     <row r="16" spans="1:16">
@@ -2143,11 +2160,11 @@
       <c r="N16" t="s">
         <v>29</v>
       </c>
-      <c r="O16" s="2">
-        <v>36.1806</v>
+      <c r="O16">
+        <v>25.4387</v>
       </c>
       <c r="P16">
-        <v>4.82438</v>
+        <v>3.39211</v>
       </c>
     </row>
     <row r="17" spans="1:16">
@@ -2194,10 +2211,10 @@
         <v>29</v>
       </c>
       <c r="O17">
-        <v>34.9452</v>
+        <v>24.5606</v>
       </c>
       <c r="P17">
-        <v>4.65963</v>
+        <v>3.27504</v>
       </c>
     </row>
     <row r="18" spans="1:16">
@@ -2244,10 +2261,10 @@
         <v>29</v>
       </c>
       <c r="O18">
-        <v>34.9414</v>
+        <v>24.5089</v>
       </c>
       <c r="P18">
-        <v>4.65915</v>
+        <v>3.26815</v>
       </c>
     </row>
     <row r="19" spans="1:16">
@@ -2294,10 +2311,10 @@
         <v>29</v>
       </c>
       <c r="O19">
-        <v>32.3595</v>
+        <v>22.4948</v>
       </c>
       <c r="P19">
-        <v>4.32169</v>
+        <v>2.9996</v>
       </c>
     </row>
     <row r="20" spans="1:16">
@@ -2344,10 +2361,10 @@
         <v>29</v>
       </c>
       <c r="O20">
-        <v>29.8798</v>
+        <v>20.6356</v>
       </c>
       <c r="P20">
-        <v>3.98426</v>
+        <v>2.7517</v>
       </c>
     </row>
     <row r="21" spans="1:16">
@@ -2394,10 +2411,10 @@
         <v>29</v>
       </c>
       <c r="O21">
-        <v>27.1946</v>
+        <v>18.5185</v>
       </c>
       <c r="P21">
-        <v>3.62624</v>
+        <v>2.46942</v>
       </c>
     </row>
     <row r="22" spans="1:16">
@@ -2444,10 +2461,10 @@
         <v>29</v>
       </c>
       <c r="O22">
-        <v>25.1805</v>
+        <v>17.0205</v>
       </c>
       <c r="P22">
-        <v>3.35768</v>
+        <v>2.26967</v>
       </c>
     </row>
     <row r="23" spans="1:16">
@@ -2494,10 +2511,10 @@
         <v>29</v>
       </c>
       <c r="O23">
-        <v>22.1358</v>
+        <v>15.3165</v>
       </c>
       <c r="P23">
-        <v>2.95171</v>
+        <v>2.04249</v>
       </c>
     </row>
     <row r="24" spans="1:16">
@@ -2544,10 +2561,10 @@
         <v>29</v>
       </c>
       <c r="O24">
-        <v>19.4481</v>
+        <v>13.8191</v>
       </c>
       <c r="P24">
-        <v>2.59337</v>
+        <v>1.84285</v>
       </c>
     </row>
     <row r="25" spans="1:16">
@@ -2594,10 +2611,10 @@
         <v>29</v>
       </c>
       <c r="O25">
-        <v>16.5563</v>
+        <v>12.3728</v>
       </c>
       <c r="P25">
-        <v>2.20779</v>
+        <v>1.64999</v>
       </c>
     </row>
     <row r="26" spans="1:16">
@@ -2644,10 +2661,10 @@
         <v>29</v>
       </c>
       <c r="O26">
-        <v>17.2273</v>
+        <v>11.8561</v>
       </c>
       <c r="P26">
-        <v>2.29726</v>
+        <v>1.58111</v>
       </c>
     </row>
     <row r="27" spans="1:16">
@@ -2694,10 +2711,10 @@
         <v>29</v>
       </c>
       <c r="O27">
-        <v>14.594</v>
+        <v>10.2041</v>
       </c>
       <c r="P27">
-        <v>1.95292</v>
+        <v>1.36084</v>
       </c>
     </row>
     <row r="28" spans="1:16">
@@ -2744,10 +2761,10 @@
         <v>29</v>
       </c>
       <c r="O28">
-        <v>12.4759</v>
+        <v>8.55532</v>
       </c>
       <c r="P28">
-        <v>1.66374</v>
+        <v>1.14101</v>
       </c>
     </row>
     <row r="29" spans="1:16">
@@ -2794,10 +2811,10 @@
         <v>29</v>
       </c>
       <c r="O29">
-        <v>9.997210000000001</v>
+        <v>6.84673</v>
       </c>
       <c r="P29">
-        <v>1.33325</v>
+        <v>0.9131860000000001</v>
       </c>
     </row>
     <row r="30" spans="1:16">
@@ -2844,10 +2861,10 @@
         <v>29</v>
       </c>
       <c r="O30">
-        <v>7.98246</v>
+        <v>5.29665</v>
       </c>
       <c r="P30">
-        <v>1.06462</v>
+        <v>0.706519</v>
       </c>
     </row>
     <row r="31" spans="1:16">
@@ -2894,10 +2911,10 @@
         <v>29</v>
       </c>
       <c r="O31">
-        <v>5.29784</v>
+        <v>3.59238</v>
       </c>
       <c r="P31">
-        <v>0.706669</v>
+        <v>0.479268</v>
       </c>
     </row>
     <row r="32" spans="1:16">
@@ -2944,10 +2961,10 @@
         <v>29</v>
       </c>
       <c r="O32">
-        <v>2.76606</v>
+        <v>1.83679</v>
       </c>
       <c r="P32">
-        <v>0.369096</v>
+        <v>0.252037</v>
       </c>
     </row>
     <row r="33" spans="1:16">
@@ -2994,10 +3011,10 @@
         <v>29</v>
       </c>
       <c r="O33">
-        <v>0.0294482</v>
+        <v>0.08040319999999999</v>
       </c>
       <c r="P33">
-        <v>0.0042354</v>
+        <v>0.0110034</v>
       </c>
     </row>
     <row r="34" spans="1:16">
@@ -3044,10 +3061,10 @@
         <v>29</v>
       </c>
       <c r="O34">
-        <v>0.0801687</v>
+        <v>0.0289182</v>
       </c>
       <c r="P34">
-        <v>0.0109695</v>
+        <v>0.00414103</v>
       </c>
     </row>
     <row r="35" spans="1:16">
@@ -3094,10 +3111,10 @@
         <v>29</v>
       </c>
       <c r="O35">
-        <v>-2.65557</v>
+        <v>-1.67513</v>
       </c>
       <c r="P35">
-        <v>-0.353793</v>
+        <v>-0.223063</v>
       </c>
     </row>
     <row r="36" spans="1:16">
@@ -3144,10 +3161,10 @@
         <v>29</v>
       </c>
       <c r="O36">
-        <v>-5.34032</v>
+        <v>-3.48164</v>
       </c>
       <c r="P36">
-        <v>-0.71175</v>
+        <v>-0.463927</v>
       </c>
     </row>
     <row r="37" spans="1:16">
@@ -3194,10 +3211,10 @@
         <v>29</v>
       </c>
       <c r="O37">
-        <v>-7.92251</v>
+        <v>-5.18569</v>
       </c>
       <c r="P37">
-        <v>-1.05604</v>
+        <v>-0.691134</v>
       </c>
     </row>
     <row r="38" spans="1:16">
@@ -3244,10 +3261,10 @@
         <v>29</v>
       </c>
       <c r="O38">
-        <v>-9.88449</v>
+        <v>-6.73475</v>
       </c>
       <c r="P38">
-        <v>-1.31765</v>
+        <v>-0.8976690000000001</v>
       </c>
     </row>
     <row r="39" spans="1:16">
@@ -3294,10 +3311,10 @@
         <v>29</v>
       </c>
       <c r="O39">
-        <v>-12.4152</v>
+        <v>-8.538690000000001</v>
       </c>
       <c r="P39">
-        <v>-1.65506</v>
+        <v>-1.13822</v>
       </c>
     </row>
     <row r="40" spans="1:16">
@@ -3344,10 +3361,10 @@
         <v>29</v>
       </c>
       <c r="O40">
-        <v>-14.5331</v>
+        <v>-10.091</v>
       </c>
       <c r="P40">
-        <v>-1.93745</v>
+        <v>-1.34518</v>
       </c>
     </row>
     <row r="41" spans="1:16">
@@ -3394,10 +3411,10 @@
         <v>29</v>
       </c>
       <c r="O41">
-        <v>-16.908</v>
+        <v>-11.8467</v>
       </c>
       <c r="P41">
-        <v>-2.25411</v>
+        <v>-1.57928</v>
       </c>
     </row>
     <row r="42" spans="1:16">
@@ -3444,10 +3461,10 @@
         <v>29</v>
       </c>
       <c r="O42">
-        <v>-16.2847</v>
+        <v>-12.3118</v>
       </c>
       <c r="P42">
-        <v>-2.17097</v>
+        <v>-1.64129</v>
       </c>
     </row>
     <row r="43" spans="1:16">
@@ -3494,10 +3511,10 @@
         <v>29</v>
       </c>
       <c r="O43">
-        <v>-19.0248</v>
+        <v>-13.7581</v>
       </c>
       <c r="P43">
-        <v>-2.53636</v>
+        <v>-1.83413</v>
       </c>
     </row>
     <row r="44" spans="1:16">
@@ -3544,10 +3561,10 @@
         <v>29</v>
       </c>
       <c r="O44">
-        <v>-21.8134</v>
+        <v>-15.1516</v>
       </c>
       <c r="P44">
-        <v>-2.90816</v>
+        <v>-2.01317</v>
       </c>
     </row>
     <row r="45" spans="1:16">
@@ -3594,10 +3611,10 @@
         <v>29</v>
       </c>
       <c r="O45">
-        <v>-24.6016</v>
+        <v>-16.6498</v>
       </c>
       <c r="P45">
-        <v>-3.27992</v>
+        <v>-2.21968</v>
       </c>
     </row>
     <row r="46" spans="1:16">
@@ -3644,10 +3661,10 @@
         <v>29</v>
       </c>
       <c r="O46">
-        <v>-26.6151</v>
+        <v>-18.0959</v>
       </c>
       <c r="P46">
-        <v>-3.54837</v>
+        <v>-2.41249</v>
       </c>
     </row>
     <row r="47" spans="1:16">
@@ -3694,10 +3711,10 @@
         <v>29</v>
       </c>
       <c r="O47">
-        <v>-29.4036</v>
+        <v>-20.0576</v>
       </c>
       <c r="P47">
-        <v>-3.92019</v>
+        <v>-2.67404</v>
       </c>
     </row>
     <row r="48" spans="1:16">
@@ -3744,10 +3761,10 @@
         <v>29</v>
       </c>
       <c r="O48">
-        <v>-31.8307</v>
+        <v>-21.9685</v>
       </c>
       <c r="P48">
-        <v>-4.2438</v>
+        <v>-2.92884</v>
       </c>
     </row>
     <row r="49" spans="1:16">
@@ -3794,10 +3811,10 @@
         <v>29</v>
       </c>
       <c r="O49">
-        <v>-34.5672</v>
+        <v>-23.9819</v>
       </c>
       <c r="P49">
-        <v>-4.60867</v>
+        <v>-3.1973</v>
       </c>
     </row>
     <row r="50" spans="1:16">
@@ -3844,10 +3861,10 @@
         <v>29</v>
       </c>
       <c r="O50">
-        <v>-34.6168</v>
+        <v>-23.982</v>
       </c>
       <c r="P50">
-        <v>-4.6153</v>
+        <v>-3.19731</v>
       </c>
     </row>
     <row r="51" spans="1:16">
@@ -3893,11 +3910,11 @@
       <c r="N51" t="s">
         <v>29</v>
       </c>
-      <c r="O51" s="3">
-        <v>-35.8582</v>
+      <c r="O51">
+        <v>-24.8083</v>
       </c>
       <c r="P51">
-        <v>-4.78079</v>
+        <v>-3.30748</v>
       </c>
     </row>
     <row r="52" spans="1:16">
@@ -3943,11 +3960,11 @@
       <c r="N52" t="s">
         <v>29</v>
       </c>
-      <c r="O52" s="3">
-        <v>-36.891</v>
+      <c r="O52">
+        <v>-25.6344</v>
       </c>
       <c r="P52">
-        <v>-4.9185</v>
+        <v>-3.41763</v>
       </c>
     </row>
     <row r="53" spans="1:16">
@@ -3993,11 +4010,11 @@
       <c r="N53" t="s">
         <v>29</v>
       </c>
-      <c r="O53" s="3">
-        <v>-38.2335</v>
+      <c r="O53">
+        <v>-26.6154</v>
       </c>
       <c r="P53">
-        <v>-5.09751</v>
+        <v>-3.54843</v>
       </c>
     </row>
     <row r="54" spans="1:16">
@@ -4043,11 +4060,11 @@
       <c r="N54" t="s">
         <v>29</v>
       </c>
-      <c r="O54" s="3">
-        <v>-38.7499</v>
+      <c r="O54">
+        <v>-27.2352</v>
       </c>
       <c r="P54">
-        <v>-5.16635</v>
+        <v>-3.63107</v>
       </c>
     </row>
     <row r="55" spans="1:16">
@@ -4093,11 +4110,11 @@
       <c r="N55" t="s">
         <v>29</v>
       </c>
-      <c r="O55" s="3">
-        <v>-40.0924</v>
+      <c r="O55">
+        <v>-28.1131</v>
       </c>
       <c r="P55">
-        <v>-5.34535</v>
+        <v>-3.74813</v>
       </c>
     </row>
     <row r="56" spans="1:16">
@@ -4143,11 +4160,11 @@
       <c r="N56" t="s">
         <v>29</v>
       </c>
-      <c r="O56" s="3">
-        <v>-41.4863</v>
+      <c r="O56">
+        <v>-28.9909</v>
       </c>
       <c r="P56">
-        <v>-5.53122</v>
+        <v>-3.86516</v>
       </c>
     </row>
     <row r="57" spans="1:16">
@@ -4193,11 +4210,11 @@
       <c r="N57" t="s">
         <v>29</v>
       </c>
-      <c r="O57" s="3">
-        <v>-42.7775</v>
+      <c r="O57">
+        <v>-29.8687</v>
       </c>
       <c r="P57">
-        <v>-5.70336</v>
+        <v>-3.9822</v>
       </c>
     </row>
     <row r="58" spans="1:16">
@@ -4243,11 +4260,11 @@
       <c r="N58" t="s">
         <v>29</v>
       </c>
-      <c r="O58" s="3">
-        <v>-41.6929</v>
+      <c r="O58">
+        <v>-29.6623</v>
       </c>
       <c r="P58">
-        <v>-5.55877</v>
+        <v>-3.95468</v>
       </c>
     </row>
     <row r="59" spans="1:16">
@@ -4293,11 +4310,11 @@
       <c r="N59" t="s">
         <v>29</v>
       </c>
-      <c r="O59" s="3">
-        <v>-43.2421</v>
+      <c r="O59">
+        <v>-30.5399</v>
       </c>
       <c r="P59">
-        <v>-5.76532</v>
+        <v>-4.0717</v>
       </c>
     </row>
     <row r="60" spans="1:16">
@@ -4343,11 +4360,11 @@
       <c r="N60" t="s">
         <v>29</v>
       </c>
-      <c r="O60" s="3">
-        <v>-44.4815</v>
+      <c r="O60">
+        <v>-31.4694</v>
       </c>
       <c r="P60">
-        <v>-5.93058</v>
+        <v>-4.19564</v>
       </c>
     </row>
     <row r="61" spans="1:16">
@@ -4393,11 +4410,11 @@
       <c r="N61" t="s">
         <v>29</v>
       </c>
-      <c r="O61" s="3">
-        <v>-45.9788</v>
+      <c r="O61">
+        <v>-32.3938</v>
       </c>
       <c r="P61">
-        <v>-6.1302</v>
+        <v>-4.31891</v>
       </c>
     </row>
     <row r="62" spans="1:16">
@@ -4443,11 +4460,11 @@
       <c r="N62" t="s">
         <v>29</v>
       </c>
-      <c r="O62" s="3">
-        <v>-46.6497</v>
+      <c r="O62">
+        <v>-32.9672</v>
       </c>
       <c r="P62">
-        <v>-6.21967</v>
+        <v>-4.39533</v>
       </c>
     </row>
     <row r="63" spans="1:16">
@@ -4493,11 +4510,11 @@
       <c r="N63" t="s">
         <v>29</v>
       </c>
-      <c r="O63" s="3">
-        <v>-48.1471</v>
+      <c r="O63">
+        <v>-33.948</v>
       </c>
       <c r="P63">
-        <v>-6.41931</v>
+        <v>-4.52611</v>
       </c>
     </row>
     <row r="64" spans="1:16">
@@ -4543,11 +4560,11 @@
       <c r="N64" t="s">
         <v>29</v>
       </c>
-      <c r="O64" s="3">
-        <v>-49.3339</v>
+      <c r="O64">
+        <v>-34.8225</v>
       </c>
       <c r="P64">
-        <v>-6.57757</v>
+        <v>-4.64273</v>
       </c>
     </row>
     <row r="65" spans="1:16">
@@ -4594,10 +4611,10 @@
         <v>29</v>
       </c>
       <c r="O65" s="3">
-        <v>-50.6776</v>
+        <v>-35.7554</v>
       </c>
       <c r="P65">
-        <v>-6.75672</v>
+        <v>-4.76709</v>
       </c>
     </row>
     <row r="66" spans="1:16">
@@ -4644,10 +4661,10 @@
         <v>165</v>
       </c>
       <c r="O66" s="2">
-        <v>64.79049999999999</v>
+        <v>48.4135</v>
       </c>
       <c r="P66">
-        <v>7.85358</v>
+        <v>5.86849</v>
       </c>
     </row>
     <row r="67" spans="1:16">
@@ -4694,10 +4711,10 @@
         <v>165</v>
       </c>
       <c r="O67" s="2">
-        <v>63.2869</v>
+        <v>47.162</v>
       </c>
       <c r="P67">
-        <v>7.67133</v>
+        <v>5.71679</v>
       </c>
     </row>
     <row r="68" spans="1:16">
@@ -4744,10 +4761,10 @@
         <v>165</v>
       </c>
       <c r="O68" s="2">
-        <v>61.1306</v>
+        <v>44.5051</v>
       </c>
       <c r="P68">
-        <v>7.40995</v>
+        <v>5.39474</v>
       </c>
     </row>
     <row r="69" spans="1:16">
@@ -4794,10 +4811,10 @@
         <v>165</v>
       </c>
       <c r="O69" s="2">
-        <v>59.1294</v>
+        <v>43.3533</v>
       </c>
       <c r="P69">
-        <v>7.16738</v>
+        <v>5.25513</v>
       </c>
     </row>
     <row r="70" spans="1:16">
@@ -4844,10 +4861,10 @@
         <v>165</v>
       </c>
       <c r="O70" s="2">
-        <v>58.3264</v>
+        <v>42.6521</v>
       </c>
       <c r="P70">
-        <v>7.07005</v>
+        <v>5.17015</v>
       </c>
     </row>
     <row r="71" spans="1:16">
@@ -4894,10 +4911,10 @@
         <v>165</v>
       </c>
       <c r="O71" s="2">
-        <v>56.4737</v>
+        <v>41.5041</v>
       </c>
       <c r="P71">
-        <v>6.84547</v>
+        <v>5.03098</v>
       </c>
     </row>
     <row r="72" spans="1:16">
@@ -4944,10 +4961,10 @@
         <v>165</v>
       </c>
       <c r="O72" s="2">
-        <v>54.9212</v>
+        <v>40.5486</v>
       </c>
       <c r="P72">
-        <v>6.65731</v>
+        <v>4.91517</v>
       </c>
     </row>
     <row r="73" spans="1:16">
@@ -4994,10 +5011,10 @@
         <v>165</v>
       </c>
       <c r="O73" s="2">
-        <v>53.3186</v>
+        <v>39.3995</v>
       </c>
       <c r="P73">
-        <v>6.46305</v>
+        <v>4.77587</v>
       </c>
     </row>
     <row r="74" spans="1:16">
@@ -5044,10 +5061,10 @@
         <v>165</v>
       </c>
       <c r="O74" s="2">
-        <v>54.6709</v>
+        <v>39.7475</v>
       </c>
       <c r="P74">
-        <v>6.62696</v>
+        <v>4.81807</v>
       </c>
     </row>
     <row r="75" spans="1:16">
@@ -5094,10 +5111,10 @@
         <v>165</v>
       </c>
       <c r="O75" s="2">
-        <v>53.1183</v>
+        <v>38.5965</v>
       </c>
       <c r="P75">
-        <v>6.43876</v>
+        <v>4.67855</v>
       </c>
     </row>
     <row r="76" spans="1:16">
@@ -5144,10 +5161,10 @@
         <v>165</v>
       </c>
       <c r="O76" s="2">
-        <v>51.6659</v>
+        <v>37.5441</v>
       </c>
       <c r="P76">
-        <v>6.2627</v>
+        <v>4.55099</v>
       </c>
     </row>
     <row r="77" spans="1:16">
@@ -5194,10 +5211,10 @@
         <v>165</v>
       </c>
       <c r="O77" s="2">
-        <v>50.0637</v>
+        <v>36.3425</v>
       </c>
       <c r="P77">
-        <v>6.06852</v>
+        <v>4.40534</v>
       </c>
     </row>
     <row r="78" spans="1:16">
@@ -5244,10 +5261,10 @@
         <v>165</v>
       </c>
       <c r="O78" s="2">
-        <v>49.3121</v>
+        <v>35.5414</v>
       </c>
       <c r="P78">
-        <v>5.97741</v>
+        <v>4.30825</v>
       </c>
     </row>
     <row r="79" spans="1:16">
@@ -5293,11 +5310,11 @@
       <c r="N79" t="s">
         <v>165</v>
       </c>
-      <c r="O79" s="2">
-        <v>47.7596</v>
+      <c r="O79">
+        <v>34.3901</v>
       </c>
       <c r="P79">
-        <v>5.78924</v>
+        <v>4.16868</v>
       </c>
     </row>
     <row r="80" spans="1:16">
@@ -5343,11 +5360,11 @@
       <c r="N80" t="s">
         <v>165</v>
       </c>
-      <c r="O80" s="2">
-        <v>46.4584</v>
+      <c r="O80">
+        <v>33.2885</v>
       </c>
       <c r="P80">
-        <v>5.63151</v>
+        <v>4.03516</v>
       </c>
     </row>
     <row r="81" spans="1:16">
@@ -5393,11 +5410,11 @@
       <c r="N81" t="s">
         <v>165</v>
       </c>
-      <c r="O81" s="2">
-        <v>45.006</v>
+      <c r="O81">
+        <v>32.0871</v>
       </c>
       <c r="P81">
-        <v>5.45545</v>
+        <v>3.88953</v>
       </c>
     </row>
     <row r="82" spans="1:16">
@@ -5443,11 +5460,11 @@
       <c r="N82" t="s">
         <v>165</v>
       </c>
-      <c r="O82" s="2">
-        <v>44.9557</v>
+      <c r="O82">
+        <v>32.087</v>
       </c>
       <c r="P82">
-        <v>5.44937</v>
+        <v>3.88952</v>
       </c>
     </row>
     <row r="83" spans="1:16">
@@ -5493,11 +5510,11 @@
       <c r="N83" t="s">
         <v>165</v>
       </c>
-      <c r="O83" s="2">
-        <v>41.4502</v>
+      <c r="O83">
+        <v>29.7342</v>
       </c>
       <c r="P83">
-        <v>5.02445</v>
+        <v>3.60433</v>
       </c>
     </row>
     <row r="84" spans="1:16">
@@ -5543,11 +5560,11 @@
       <c r="N84" t="s">
         <v>165</v>
       </c>
-      <c r="O84" s="2">
-        <v>38.245</v>
+      <c r="O84">
+        <v>27.4314</v>
       </c>
       <c r="P84">
-        <v>4.63593</v>
+        <v>3.32521</v>
       </c>
     </row>
     <row r="85" spans="1:16">
@@ -5594,10 +5611,10 @@
         <v>165</v>
       </c>
       <c r="O85">
-        <v>34.7906</v>
+        <v>24.9781</v>
       </c>
       <c r="P85">
-        <v>4.21723</v>
+        <v>3.02783</v>
       </c>
     </row>
     <row r="86" spans="1:16">
@@ -5644,10 +5661,10 @@
         <v>165</v>
       </c>
       <c r="O86">
-        <v>32.4886</v>
+        <v>23.025</v>
       </c>
       <c r="P86">
-        <v>3.93819</v>
+        <v>2.79109</v>
       </c>
     </row>
     <row r="87" spans="1:16">
@@ -5694,10 +5711,10 @@
         <v>165</v>
       </c>
       <c r="O87">
-        <v>29.0332</v>
+        <v>20.6717</v>
       </c>
       <c r="P87">
-        <v>3.51936</v>
+        <v>2.50584</v>
       </c>
     </row>
     <row r="88" spans="1:16">
@@ -5744,10 +5761,10 @@
         <v>165</v>
       </c>
       <c r="O88">
-        <v>25.6289</v>
+        <v>18.4693</v>
       </c>
       <c r="P88">
-        <v>3.10672</v>
+        <v>2.24485</v>
       </c>
     </row>
     <row r="89" spans="1:16">
@@ -5794,10 +5811,10 @@
         <v>165</v>
       </c>
       <c r="O89">
-        <v>22.1237</v>
+        <v>16.2153</v>
       </c>
       <c r="P89">
-        <v>2.68186</v>
+        <v>1.96568</v>
       </c>
     </row>
     <row r="90" spans="1:16">
@@ -5844,10 +5861,10 @@
         <v>165</v>
       </c>
       <c r="O90">
-        <v>22.925</v>
+        <v>15.5644</v>
       </c>
       <c r="P90">
-        <v>2.77898</v>
+        <v>1.88678</v>
       </c>
     </row>
     <row r="91" spans="1:16">
@@ -5894,10 +5911,10 @@
         <v>165</v>
       </c>
       <c r="O91">
-        <v>19.5199</v>
+        <v>13.1107</v>
       </c>
       <c r="P91">
-        <v>2.36624</v>
+        <v>1.58936</v>
       </c>
     </row>
     <row r="92" spans="1:16">
@@ -5944,10 +5961,10 @@
         <v>165</v>
       </c>
       <c r="O92">
-        <v>16.1653</v>
+        <v>10.7072</v>
       </c>
       <c r="P92">
-        <v>1.95961</v>
+        <v>1.29802</v>
       </c>
     </row>
     <row r="93" spans="1:16">
@@ -5994,10 +6011,10 @@
         <v>165</v>
       </c>
       <c r="O93">
-        <v>12.51</v>
+        <v>8.25394</v>
       </c>
       <c r="P93">
-        <v>1.51656</v>
+        <v>1.00066</v>
       </c>
     </row>
     <row r="94" spans="1:16">
@@ -6044,10 +6061,10 @@
         <v>165</v>
       </c>
       <c r="O94">
-        <v>9.506640000000001</v>
+        <v>6.36319</v>
       </c>
       <c r="P94">
-        <v>1.1525</v>
+        <v>0.771471</v>
       </c>
     </row>
     <row r="95" spans="1:16">
@@ -6094,10 +6111,10 @@
         <v>165</v>
       </c>
       <c r="O95">
-        <v>6.30109</v>
+        <v>4.29948</v>
       </c>
       <c r="P95">
-        <v>0.76395</v>
+        <v>0.5213410000000001</v>
       </c>
     </row>
     <row r="96" spans="1:16">
@@ -6144,10 +6161,10 @@
         <v>165</v>
       </c>
       <c r="O96">
-        <v>32.4886</v>
+        <v>23.025</v>
       </c>
       <c r="P96">
-        <v>3.93819</v>
+        <v>2.79109</v>
       </c>
     </row>
     <row r="97" spans="1:16">
@@ -6194,10 +6211,10 @@
         <v>165</v>
       </c>
       <c r="O97">
-        <v>29.0332</v>
+        <v>20.6717</v>
       </c>
       <c r="P97">
-        <v>3.51936</v>
+        <v>2.50584</v>
       </c>
     </row>
     <row r="98" spans="1:16">
@@ -6244,10 +6261,10 @@
         <v>165</v>
       </c>
       <c r="O98">
-        <v>25.6289</v>
+        <v>18.4693</v>
       </c>
       <c r="P98">
-        <v>3.10672</v>
+        <v>2.24485</v>
       </c>
     </row>
     <row r="99" spans="1:16">
@@ -6294,10 +6311,10 @@
         <v>165</v>
       </c>
       <c r="O99">
-        <v>22.1237</v>
+        <v>16.2153</v>
       </c>
       <c r="P99">
-        <v>2.68186</v>
+        <v>1.96568</v>
       </c>
     </row>
     <row r="100" spans="1:16">
@@ -6344,10 +6361,10 @@
         <v>165</v>
       </c>
       <c r="O100">
-        <v>22.925</v>
+        <v>15.5644</v>
       </c>
       <c r="P100">
-        <v>2.77898</v>
+        <v>1.88678</v>
       </c>
     </row>
     <row r="101" spans="1:16">
@@ -6394,10 +6411,10 @@
         <v>165</v>
       </c>
       <c r="O101">
-        <v>19.5199</v>
+        <v>13.1107</v>
       </c>
       <c r="P101">
-        <v>2.36624</v>
+        <v>1.58936</v>
       </c>
     </row>
     <row r="102" spans="1:16">
@@ -6444,10 +6461,10 @@
         <v>165</v>
       </c>
       <c r="O102">
-        <v>16.1653</v>
+        <v>10.7072</v>
       </c>
       <c r="P102">
-        <v>1.95961</v>
+        <v>1.29802</v>
       </c>
     </row>
     <row r="103" spans="1:16">
@@ -6494,10 +6511,10 @@
         <v>165</v>
       </c>
       <c r="O103">
-        <v>12.51</v>
+        <v>8.25394</v>
       </c>
       <c r="P103">
-        <v>1.51656</v>
+        <v>1.00066</v>
       </c>
     </row>
     <row r="104" spans="1:16">
@@ -6544,10 +6561,10 @@
         <v>165</v>
       </c>
       <c r="O104">
-        <v>9.506640000000001</v>
+        <v>6.36319</v>
       </c>
       <c r="P104">
-        <v>1.1525</v>
+        <v>0.771471</v>
       </c>
     </row>
     <row r="105" spans="1:16">
@@ -6594,10 +6611,10 @@
         <v>165</v>
       </c>
       <c r="O105">
-        <v>6.30109</v>
+        <v>4.29948</v>
       </c>
       <c r="P105">
-        <v>0.76395</v>
+        <v>0.5213410000000001</v>
       </c>
     </row>
     <row r="106" spans="1:16">
@@ -6644,10 +6661,10 @@
         <v>165</v>
       </c>
       <c r="O106">
-        <v>3.24784</v>
+        <v>2.14766</v>
       </c>
       <c r="P106">
-        <v>0.393863</v>
+        <v>0.260502</v>
       </c>
     </row>
     <row r="107" spans="1:16">
@@ -6694,10 +6711,10 @@
         <v>165</v>
       </c>
       <c r="O107">
-        <v>-0.00473412</v>
+        <v>0.0448954</v>
       </c>
       <c r="P107">
-        <v>-0.000385116</v>
+        <v>0.00562796</v>
       </c>
     </row>
     <row r="108" spans="1:16">
@@ -6744,10 +6761,10 @@
         <v>165</v>
       </c>
       <c r="O108">
-        <v>-0.00497337</v>
+        <v>-0.00474354</v>
       </c>
       <c r="P108">
-        <v>-0.000409792</v>
+        <v>-0.000388373</v>
       </c>
     </row>
     <row r="109" spans="1:16">
@@ -6794,10 +6811,10 @@
         <v>165</v>
       </c>
       <c r="O109">
-        <v>-3.2083</v>
+        <v>-2.15761</v>
       </c>
       <c r="P109">
-        <v>-0.388691</v>
+        <v>-0.26134</v>
       </c>
     </row>
     <row r="110" spans="1:16">
@@ -6844,10 +6861,10 @@
         <v>165</v>
       </c>
       <c r="O110">
-        <v>-6.21143</v>
+        <v>-4.2092</v>
       </c>
       <c r="P110">
-        <v>-0.752714</v>
+        <v>-0.51001</v>
       </c>
     </row>
     <row r="111" spans="1:16">
@@ -6894,10 +6911,10 @@
         <v>165</v>
       </c>
       <c r="O111">
-        <v>-9.6152</v>
+        <v>-6.31153</v>
       </c>
       <c r="P111">
-        <v>-1.16528</v>
+        <v>-0.7648509999999999</v>
       </c>
     </row>
     <row r="112" spans="1:16">
@@ -6944,10 +6961,10 @@
         <v>165</v>
       </c>
       <c r="O112">
-        <v>-12.568</v>
+        <v>-8.36379</v>
       </c>
       <c r="P112">
-        <v>-1.52323</v>
+        <v>-1.0136</v>
       </c>
     </row>
     <row r="113" spans="1:16">
@@ -6994,10 +7011,10 @@
         <v>165</v>
       </c>
       <c r="O113">
-        <v>-16.171</v>
+        <v>-10.716</v>
       </c>
       <c r="P113">
-        <v>-1.95993</v>
+        <v>-1.29872</v>
       </c>
     </row>
     <row r="114" spans="1:16">
@@ -7044,10 +7061,10 @@
         <v>165</v>
       </c>
       <c r="O114">
-        <v>-19.5749</v>
+        <v>-13.1187</v>
       </c>
       <c r="P114">
-        <v>-2.36658</v>
+        <v>-1.58996</v>
       </c>
     </row>
     <row r="115" spans="1:16">
@@ -7094,10 +7111,10 @@
         <v>165</v>
       </c>
       <c r="O115">
-        <v>-22.979</v>
+        <v>-15.5713</v>
       </c>
       <c r="P115">
-        <v>-2.78515</v>
+        <v>-1.88725</v>
       </c>
     </row>
     <row r="116" spans="1:16">
@@ -7144,10 +7161,10 @@
         <v>165</v>
       </c>
       <c r="O116">
-        <v>-22.2285</v>
+        <v>-16.2718</v>
       </c>
       <c r="P116">
-        <v>-2.69417</v>
+        <v>-1.97215</v>
       </c>
     </row>
     <row r="117" spans="1:16">
@@ -7194,10 +7211,10 @@
         <v>165</v>
       </c>
       <c r="O117">
-        <v>-25.7312</v>
+        <v>-18.6245</v>
       </c>
       <c r="P117">
-        <v>-3.11876</v>
+        <v>-2.25733</v>
       </c>
     </row>
     <row r="118" spans="1:16">
@@ -7244,10 +7261,10 @@
         <v>165</v>
       </c>
       <c r="O118">
-        <v>-28.9842</v>
+        <v>-20.7771</v>
       </c>
       <c r="P118">
-        <v>-3.51304</v>
+        <v>-2.51825</v>
       </c>
     </row>
     <row r="119" spans="1:16">
@@ -7294,10 +7311,10 @@
         <v>165</v>
       </c>
       <c r="O119">
-        <v>-32.4361</v>
+        <v>-23.0292</v>
       </c>
       <c r="P119">
-        <v>-3.93146</v>
+        <v>-2.79122</v>
       </c>
     </row>
     <row r="120" spans="1:16">
@@ -7344,10 +7361,10 @@
         <v>165</v>
       </c>
       <c r="O120">
-        <v>-34.7867</v>
+        <v>-25.0317</v>
       </c>
       <c r="P120">
-        <v>-4.21639</v>
+        <v>-3.03396</v>
       </c>
     </row>
     <row r="121" spans="1:16">
@@ -7393,11 +7410,11 @@
       <c r="N121" t="s">
         <v>165</v>
       </c>
-      <c r="O121" s="3">
-        <v>-38.1398</v>
+      <c r="O121">
+        <v>-27.4317</v>
       </c>
       <c r="P121">
-        <v>-4.62282</v>
+        <v>-3.31901</v>
       </c>
     </row>
     <row r="122" spans="1:16">
@@ -7443,11 +7460,11 @@
       <c r="N122" t="s">
         <v>165</v>
       </c>
-      <c r="O122" s="3">
-        <v>-41.4419</v>
+      <c r="O122">
+        <v>-29.6846</v>
       </c>
       <c r="P122">
-        <v>-5.02307</v>
+        <v>-3.59795</v>
       </c>
     </row>
     <row r="123" spans="1:16">
@@ -7493,11 +7510,11 @@
       <c r="N123" t="s">
         <v>165</v>
       </c>
-      <c r="O123" s="3">
-        <v>-45.0933</v>
+      <c r="O123">
+        <v>-32.036</v>
       </c>
       <c r="P123">
-        <v>-5.46568</v>
+        <v>-3.88297</v>
       </c>
     </row>
     <row r="124" spans="1:16">
@@ -7543,11 +7560,11 @@
       <c r="N124" t="s">
         <v>165</v>
       </c>
-      <c r="O124" s="3">
-        <v>-45.0762</v>
+      <c r="O124">
+        <v>-32.0831</v>
       </c>
       <c r="P124">
-        <v>-5.45975</v>
+        <v>-3.88868</v>
       </c>
     </row>
     <row r="125" spans="1:16">
@@ -7593,11 +7610,11 @@
       <c r="N125" t="s">
         <v>165</v>
       </c>
-      <c r="O125" s="3">
-        <v>-46.7956</v>
+      <c r="O125">
+        <v>-33.2865</v>
       </c>
       <c r="P125">
-        <v>-5.67201</v>
+        <v>-4.03454</v>
       </c>
     </row>
     <row r="126" spans="1:16">
@@ -7643,11 +7660,11 @@
       <c r="N126" t="s">
         <v>165</v>
       </c>
-      <c r="O126" s="3">
-        <v>-48.3464</v>
+      <c r="O126">
+        <v>-34.3374</v>
       </c>
       <c r="P126">
-        <v>-5.85997</v>
+        <v>-4.16191</v>
       </c>
     </row>
     <row r="127" spans="1:16">
@@ -7694,10 +7711,10 @@
         <v>165</v>
       </c>
       <c r="O127" s="3">
-        <v>-50.0475</v>
+        <v>-35.588</v>
       </c>
       <c r="P127">
-        <v>-6.06617</v>
+        <v>-4.31351</v>
       </c>
     </row>
     <row r="128" spans="1:16">
@@ -7744,10 +7761,10 @@
         <v>165</v>
       </c>
       <c r="O128" s="3">
-        <v>-50.8481</v>
+        <v>-36.3384</v>
       </c>
       <c r="P128">
-        <v>-6.16322</v>
+        <v>-4.40448</v>
       </c>
     </row>
     <row r="129" spans="1:16">
@@ -7794,10 +7811,10 @@
         <v>165</v>
       </c>
       <c r="O129" s="3">
-        <v>-52.5494</v>
+        <v>-37.5394</v>
       </c>
       <c r="P129">
-        <v>-6.36943</v>
+        <v>-4.55004</v>
       </c>
     </row>
     <row r="130" spans="1:16">
@@ -7844,10 +7861,10 @@
         <v>165</v>
       </c>
       <c r="O130" s="3">
-        <v>-54.1002</v>
+        <v>-38.6399</v>
       </c>
       <c r="P130">
-        <v>-6.55741</v>
+        <v>-4.68344</v>
       </c>
     </row>
     <row r="131" spans="1:16">
@@ -7894,10 +7911,10 @@
         <v>165</v>
       </c>
       <c r="O131" s="3">
-        <v>-55.7509</v>
+        <v>-39.7909</v>
       </c>
       <c r="P131">
-        <v>-6.7575</v>
+        <v>-4.82295</v>
       </c>
     </row>
     <row r="132" spans="1:16">
@@ -7944,10 +7961,10 @@
         <v>165</v>
       </c>
       <c r="O132" s="3">
-        <v>-54.3002</v>
+        <v>-39.4405</v>
       </c>
       <c r="P132">
-        <v>-6.58165</v>
+        <v>-4.78048</v>
       </c>
     </row>
     <row r="133" spans="1:16">
@@ -7994,10 +8011,10 @@
         <v>165</v>
       </c>
       <c r="O133" s="3">
-        <v>-56.0004</v>
+        <v>-40.6415</v>
       </c>
       <c r="P133">
-        <v>-6.78775</v>
+        <v>-4.92605</v>
       </c>
     </row>
     <row r="134" spans="1:16">
@@ -8044,10 +8061,10 @@
         <v>165</v>
       </c>
       <c r="O134" s="3">
-        <v>-57.5013</v>
+        <v>-41.7922</v>
       </c>
       <c r="P134">
-        <v>-6.96967</v>
+        <v>-5.06553</v>
       </c>
     </row>
     <row r="135" spans="1:16">
@@ -8094,10 +8111,10 @@
         <v>165</v>
       </c>
       <c r="O135" s="3">
-        <v>-59.1518</v>
+        <v>-42.9431</v>
       </c>
       <c r="P135">
-        <v>-7.16973</v>
+        <v>-5.20504</v>
       </c>
     </row>
     <row r="136" spans="1:16">
@@ -8144,10 +8161,10 @@
         <v>165</v>
       </c>
       <c r="O136" s="3">
-        <v>-59.9517</v>
+        <v>-43.6934</v>
       </c>
       <c r="P136">
-        <v>-7.26668</v>
+        <v>-5.29598</v>
       </c>
     </row>
     <row r="137" spans="1:16">
@@ -8194,10 +8211,10 @@
         <v>165</v>
       </c>
       <c r="O137" s="3">
-        <v>-61.6011</v>
+        <v>-44.9944</v>
       </c>
       <c r="P137">
-        <v>-7.46662</v>
+        <v>-5.45368</v>
       </c>
     </row>
     <row r="138" spans="1:16">
@@ -8244,10 +8261,10 @@
         <v>165</v>
       </c>
       <c r="O138" s="3">
-        <v>-62.9298</v>
+        <v>-46.1451</v>
       </c>
       <c r="P138">
-        <v>-7.62767</v>
+        <v>-5.59315</v>
       </c>
     </row>
     <row r="139" spans="1:16">
@@ -8294,10 +8311,10 @@
         <v>165</v>
       </c>
       <c r="O139" s="3">
-        <v>-64.8019</v>
+        <v>-47.4959</v>
       </c>
       <c r="P139">
-        <v>-7.85459</v>
+        <v>-5.7569</v>
       </c>
     </row>
     <row r="140" spans="1:16">
@@ -8343,11 +8360,11 @@
       <c r="N140" t="s">
         <v>249</v>
       </c>
-      <c r="O140" s="2">
-        <v>39.442</v>
+      <c r="O140">
+        <v>28.3224</v>
       </c>
       <c r="P140">
-        <v>5.84382</v>
+        <v>4.19654</v>
       </c>
     </row>
     <row r="141" spans="1:16">
@@ -8393,11 +8410,11 @@
       <c r="N141" t="s">
         <v>249</v>
       </c>
-      <c r="O141" s="2">
-        <v>38.5125</v>
+      <c r="O141">
+        <v>27.5989</v>
       </c>
       <c r="P141">
-        <v>5.70611</v>
+        <v>4.08935</v>
       </c>
     </row>
     <row r="142" spans="1:16">
@@ -8443,11 +8460,11 @@
       <c r="N142" t="s">
         <v>249</v>
       </c>
-      <c r="O142" s="2">
-        <v>36.2874</v>
+      <c r="O142">
+        <v>26.8236</v>
       </c>
       <c r="P142">
-        <v>5.37652</v>
+        <v>3.98161</v>
       </c>
     </row>
     <row r="143" spans="1:16">
@@ -8493,11 +8510,11 @@
       <c r="N143" t="s">
         <v>249</v>
       </c>
-      <c r="O143" s="2">
-        <v>35.3029</v>
+      <c r="O143">
+        <v>26.3028</v>
       </c>
       <c r="P143">
-        <v>5.23061</v>
+        <v>3.89732</v>
       </c>
     </row>
     <row r="144" spans="1:16">
@@ -8544,10 +8561,10 @@
         <v>249</v>
       </c>
       <c r="O144">
-        <v>34.9347</v>
+        <v>25.7354</v>
       </c>
       <c r="P144">
-        <v>5.17624</v>
+        <v>3.81328</v>
       </c>
     </row>
     <row r="145" spans="1:16">
@@ -8594,10 +8611,10 @@
         <v>249</v>
       </c>
       <c r="O145">
-        <v>33.9057</v>
+        <v>25.013</v>
       </c>
       <c r="P145">
-        <v>5.03077</v>
+        <v>3.71369</v>
       </c>
     </row>
     <row r="146" spans="1:16">
@@ -8644,10 +8661,10 @@
         <v>249</v>
       </c>
       <c r="O146">
-        <v>33.231</v>
+        <v>24.3936</v>
       </c>
       <c r="P146">
-        <v>4.92375</v>
+        <v>3.62189</v>
       </c>
     </row>
     <row r="147" spans="1:16">
@@ -8694,10 +8711,10 @@
         <v>249</v>
       </c>
       <c r="O147">
-        <v>32.3534</v>
+        <v>23.7715</v>
       </c>
       <c r="P147">
-        <v>4.80124</v>
+        <v>3.5224</v>
       </c>
     </row>
     <row r="148" spans="1:16">
@@ -8744,10 +8761,10 @@
         <v>249</v>
       </c>
       <c r="O148">
-        <v>32.9312</v>
+        <v>23.9274</v>
       </c>
       <c r="P148">
-        <v>4.87924</v>
+        <v>3.54547</v>
       </c>
     </row>
     <row r="149" spans="1:16">
@@ -8794,10 +8811,10 @@
         <v>249</v>
       </c>
       <c r="O149">
-        <v>32.0957</v>
+        <v>23.2585</v>
       </c>
       <c r="P149">
-        <v>4.76302</v>
+        <v>3.45341</v>
       </c>
     </row>
     <row r="150" spans="1:16">
@@ -8844,10 +8861,10 @@
         <v>249</v>
       </c>
       <c r="O150">
-        <v>31.3715</v>
+        <v>22.6358</v>
       </c>
       <c r="P150">
-        <v>4.64832</v>
+        <v>3.35414</v>
       </c>
     </row>
     <row r="151" spans="1:16">
@@ -8894,10 +8911,10 @@
         <v>249</v>
       </c>
       <c r="O151">
-        <v>30.3495</v>
+        <v>22.1708</v>
       </c>
       <c r="P151">
-        <v>4.49681</v>
+        <v>3.2852</v>
       </c>
     </row>
     <row r="152" spans="1:16">
@@ -8944,10 +8961,10 @@
         <v>249</v>
       </c>
       <c r="O152">
-        <v>29.925</v>
+        <v>21.8092</v>
       </c>
       <c r="P152">
-        <v>4.43409</v>
+        <v>3.23165</v>
       </c>
     </row>
     <row r="153" spans="1:16">
@@ -8994,10 +9011,10 @@
         <v>249</v>
       </c>
       <c r="O153">
-        <v>29.005</v>
+        <v>21.1896</v>
       </c>
       <c r="P153">
-        <v>4.2976</v>
+        <v>3.13986</v>
       </c>
     </row>
     <row r="154" spans="1:16">
@@ -9044,10 +9061,10 @@
         <v>249</v>
       </c>
       <c r="O154">
-        <v>28.2286</v>
+        <v>20.4771</v>
       </c>
       <c r="P154">
-        <v>4.18259</v>
+        <v>3.03422</v>
       </c>
     </row>
     <row r="155" spans="1:16">
@@ -9094,10 +9111,10 @@
         <v>249</v>
       </c>
       <c r="O155">
-        <v>27.2391</v>
+        <v>19.9557</v>
       </c>
       <c r="P155">
-        <v>4.03611</v>
+        <v>2.95696</v>
       </c>
     </row>
     <row r="156" spans="1:16">
@@ -9144,10 +9161,10 @@
         <v>249</v>
       </c>
       <c r="O156">
-        <v>27.2394</v>
+        <v>19.7948</v>
       </c>
       <c r="P156">
-        <v>4.03616</v>
+        <v>2.9332</v>
       </c>
     </row>
     <row r="157" spans="1:16">
@@ -9194,10 +9211,10 @@
         <v>249</v>
       </c>
       <c r="O157">
-        <v>25.0676</v>
+        <v>18.5536</v>
       </c>
       <c r="P157">
-        <v>3.71439</v>
+        <v>2.74932</v>
       </c>
     </row>
     <row r="158" spans="1:16">
@@ -9244,10 +9261,10 @@
         <v>249</v>
       </c>
       <c r="O158">
-        <v>23.216</v>
+        <v>17.3136</v>
       </c>
       <c r="P158">
-        <v>3.44015</v>
+        <v>2.56562</v>
       </c>
     </row>
     <row r="159" spans="1:16">
@@ -9294,10 +9311,10 @@
         <v>249</v>
       </c>
       <c r="O159">
-        <v>21.2419</v>
+        <v>15.9171</v>
       </c>
       <c r="P159">
-        <v>3.14768</v>
+        <v>2.35874</v>
       </c>
     </row>
     <row r="160" spans="1:16">
@@ -9344,10 +9361,10 @@
         <v>249</v>
       </c>
       <c r="O160">
-        <v>20.1063</v>
+        <v>14.9444</v>
       </c>
       <c r="P160">
-        <v>2.98677</v>
+        <v>2.21457</v>
       </c>
     </row>
     <row r="161" spans="1:16">
@@ -9394,10 +9411,10 @@
         <v>249</v>
       </c>
       <c r="O161">
-        <v>18.0885</v>
+        <v>13.4888</v>
       </c>
       <c r="P161">
-        <v>2.68042</v>
+        <v>1.99901</v>
       </c>
     </row>
     <row r="162" spans="1:16">
@@ -9444,10 +9461,10 @@
         <v>249</v>
       </c>
       <c r="O162">
-        <v>16.2382</v>
+        <v>12.1958</v>
       </c>
       <c r="P162">
-        <v>2.40621</v>
+        <v>1.80737</v>
       </c>
     </row>
     <row r="163" spans="1:16">
@@ -9494,10 +9511,10 @@
         <v>249</v>
       </c>
       <c r="O163">
-        <v>14.1083</v>
+        <v>10.646</v>
       </c>
       <c r="P163">
-        <v>2.09074</v>
+        <v>1.5778</v>
       </c>
     </row>
     <row r="164" spans="1:16">
@@ -9544,10 +9561,10 @@
         <v>249</v>
       </c>
       <c r="O164">
-        <v>15.4535</v>
+        <v>10.6458</v>
       </c>
       <c r="P164">
-        <v>2.29008</v>
+        <v>1.57766</v>
       </c>
     </row>
     <row r="165" spans="1:16">
@@ -9594,10 +9611,10 @@
         <v>249</v>
       </c>
       <c r="O165">
-        <v>13.2814</v>
+        <v>9.002280000000001</v>
       </c>
       <c r="P165">
-        <v>1.96824</v>
+        <v>1.33431</v>
       </c>
     </row>
     <row r="166" spans="1:16">
@@ -9644,10 +9661,10 @@
         <v>249</v>
       </c>
       <c r="O166">
-        <v>11.2655</v>
+        <v>7.38952</v>
       </c>
       <c r="P166">
-        <v>1.66959</v>
+        <v>1.09536</v>
       </c>
     </row>
     <row r="167" spans="1:16">
@@ -9694,10 +9711,10 @@
         <v>249</v>
       </c>
       <c r="O167">
-        <v>8.7843</v>
+        <v>5.78687</v>
       </c>
       <c r="P167">
-        <v>1.30199</v>
+        <v>0.857922</v>
       </c>
     </row>
     <row r="168" spans="1:16">
@@ -9744,10 +9761,10 @@
         <v>249</v>
       </c>
       <c r="O168">
-        <v>7.02718</v>
+        <v>4.49597</v>
       </c>
       <c r="P168">
-        <v>1.04167</v>
+        <v>0.674089</v>
       </c>
     </row>
     <row r="169" spans="1:16">
@@ -9794,10 +9811,10 @@
         <v>249</v>
       </c>
       <c r="O169">
-        <v>4.59749</v>
+        <v>3.00324</v>
       </c>
       <c r="P169">
-        <v>0.6817220000000001</v>
+        <v>0.445466</v>
       </c>
     </row>
     <row r="170" spans="1:16">
@@ -9844,10 +9861,10 @@
         <v>249</v>
       </c>
       <c r="O170">
-        <v>2.32435</v>
+        <v>1.65142</v>
       </c>
       <c r="P170">
-        <v>0.344964</v>
+        <v>0.245276</v>
       </c>
     </row>
     <row r="171" spans="1:16">
@@ -9894,10 +9911,10 @@
         <v>249</v>
       </c>
       <c r="O171">
-        <v>0.101108</v>
+        <v>0.0498098</v>
       </c>
       <c r="P171">
-        <v>0.0155834</v>
+        <v>0.007972440000000001</v>
       </c>
     </row>
     <row r="172" spans="1:16">
@@ -9944,10 +9961,10 @@
         <v>249</v>
       </c>
       <c r="O172">
-        <v>0.101619</v>
+        <v>0.102028</v>
       </c>
       <c r="P172">
-        <v>0.0156737</v>
+        <v>0.0157204</v>
       </c>
     </row>
     <row r="173" spans="1:16">
@@ -9994,10 +10011,10 @@
         <v>249</v>
       </c>
       <c r="O173">
-        <v>-2.22399</v>
+        <v>-1.39709</v>
       </c>
       <c r="P173">
-        <v>-0.328836</v>
+        <v>-0.206368</v>
       </c>
     </row>
     <row r="174" spans="1:16">
@@ -10044,10 +10061,10 @@
         <v>249</v>
       </c>
       <c r="O174">
-        <v>-4.29067</v>
+        <v>-2.79213</v>
       </c>
       <c r="P174">
-        <v>-0.635068</v>
+        <v>-0.413003</v>
       </c>
     </row>
     <row r="175" spans="1:16">
@@ -10094,10 +10111,10 @@
         <v>249</v>
       </c>
       <c r="O175">
-        <v>-6.81563</v>
+        <v>-4.34276</v>
       </c>
       <c r="P175">
-        <v>-1.00918</v>
+        <v>-0.642741</v>
       </c>
     </row>
     <row r="176" spans="1:16">
@@ -10144,10 +10161,10 @@
         <v>249</v>
       </c>
       <c r="O176">
-        <v>-8.269640000000001</v>
+        <v>-5.58313</v>
       </c>
       <c r="P176">
-        <v>-1.2245</v>
+        <v>-0.826518</v>
       </c>
     </row>
     <row r="177" spans="1:16">
@@ -10194,10 +10211,10 @@
         <v>249</v>
       </c>
       <c r="O177">
-        <v>-10.4362</v>
+        <v>-7.18472</v>
       </c>
       <c r="P177">
-        <v>-1.5455</v>
+        <v>-1.06375</v>
       </c>
     </row>
     <row r="178" spans="1:16">
@@ -10244,10 +10261,10 @@
         <v>249</v>
       </c>
       <c r="O178">
-        <v>-12.2996</v>
+        <v>-8.527200000000001</v>
       </c>
       <c r="P178">
-        <v>-1.82153</v>
+        <v>-1.2627</v>
       </c>
     </row>
     <row r="179" spans="1:16">
@@ -10294,10 +10311,10 @@
         <v>249</v>
       </c>
       <c r="O179">
-        <v>-14.3147</v>
+        <v>-9.819419999999999</v>
       </c>
       <c r="P179">
-        <v>-2.1201</v>
+        <v>-1.45411</v>
       </c>
     </row>
     <row r="180" spans="1:16">
@@ -10344,10 +10361,10 @@
         <v>249</v>
       </c>
       <c r="O180">
-        <v>-13.2736</v>
+        <v>-9.8187</v>
       </c>
       <c r="P180">
-        <v>-1.96586</v>
+        <v>-1.45401</v>
       </c>
     </row>
     <row r="181" spans="1:16">
@@ -10394,10 +10411,10 @@
         <v>249</v>
       </c>
       <c r="O181">
-        <v>-15.1924</v>
+        <v>-11.2135</v>
       </c>
       <c r="P181">
-        <v>-2.25007</v>
+        <v>-1.66061</v>
       </c>
     </row>
     <row r="182" spans="1:16">
@@ -10444,10 +10461,10 @@
         <v>249</v>
       </c>
       <c r="O182">
-        <v>-16.8901</v>
+        <v>-12.6094</v>
       </c>
       <c r="P182">
-        <v>-2.50169</v>
+        <v>-1.86742</v>
       </c>
     </row>
     <row r="183" spans="1:16">
@@ -10494,10 +10511,10 @@
         <v>249</v>
       </c>
       <c r="O183">
-        <v>-18.7579</v>
+        <v>-13.9898</v>
       </c>
       <c r="P183">
-        <v>-2.77831</v>
+        <v>-2.07197</v>
       </c>
     </row>
     <row r="184" spans="1:16">
@@ -10544,10 +10561,10 @@
         <v>249</v>
       </c>
       <c r="O184">
-        <v>-20.2048</v>
+        <v>-14.8831</v>
       </c>
       <c r="P184">
-        <v>-2.99266</v>
+        <v>-2.20426</v>
       </c>
     </row>
     <row r="185" spans="1:16">
@@ -10594,10 +10611,10 @@
         <v>249</v>
       </c>
       <c r="O185">
-        <v>-22.2193</v>
+        <v>-16.0714</v>
       </c>
       <c r="P185">
-        <v>-3.29112</v>
+        <v>-2.38032</v>
       </c>
     </row>
     <row r="186" spans="1:16">
@@ -10644,10 +10661,10 @@
         <v>249</v>
       </c>
       <c r="O186">
-        <v>-24.1837</v>
+        <v>-17.2084</v>
       </c>
       <c r="P186">
-        <v>-3.5821</v>
+        <v>-2.54872</v>
       </c>
     </row>
     <row r="187" spans="1:16">
@@ -10694,10 +10711,10 @@
         <v>249</v>
       </c>
       <c r="O187">
-        <v>-26.3467</v>
+        <v>-18.551</v>
       </c>
       <c r="P187">
-        <v>-3.90264</v>
+        <v>-2.74765</v>
       </c>
     </row>
     <row r="188" spans="1:16">
@@ -10744,10 +10761,10 @@
         <v>249</v>
       </c>
       <c r="O188">
-        <v>-26.4483</v>
+        <v>-18.6029</v>
       </c>
       <c r="P188">
-        <v>-3.91771</v>
+        <v>-2.75532</v>
       </c>
     </row>
     <row r="189" spans="1:16">
@@ -10794,10 +10811,10 @@
         <v>249</v>
       </c>
       <c r="O189">
-        <v>-27.482</v>
+        <v>-19.2754</v>
       </c>
       <c r="P189">
-        <v>-4.07085</v>
+        <v>-2.85498</v>
       </c>
     </row>
     <row r="190" spans="1:16">
@@ -10844,10 +10861,10 @@
         <v>249</v>
       </c>
       <c r="O190">
-        <v>-28.3117</v>
+        <v>-20.0392</v>
       </c>
       <c r="P190">
-        <v>-4.18703</v>
+        <v>-2.96817</v>
       </c>
     </row>
     <row r="191" spans="1:16">
@@ -10894,10 +10911,10 @@
         <v>249</v>
       </c>
       <c r="O191">
-        <v>-29.4553</v>
+        <v>-20.7738</v>
       </c>
       <c r="P191">
-        <v>-4.36306</v>
+        <v>-3.07696</v>
       </c>
     </row>
     <row r="192" spans="1:16">
@@ -10944,10 +10961,10 @@
         <v>249</v>
       </c>
       <c r="O192">
-        <v>-30.012</v>
+        <v>-21.2916</v>
       </c>
       <c r="P192">
-        <v>-4.44559</v>
+        <v>-3.15367</v>
       </c>
     </row>
     <row r="193" spans="1:16">
@@ -10994,10 +11011,10 @@
         <v>249</v>
       </c>
       <c r="O193">
-        <v>-31.058</v>
+        <v>-22.1703</v>
       </c>
       <c r="P193">
-        <v>-4.60053</v>
+        <v>-3.28389</v>
       </c>
     </row>
     <row r="194" spans="1:16">
@@ -11043,16 +11060,16 @@
       <c r="N194" t="s">
         <v>249</v>
       </c>
-      <c r="O194">
-        <v>-31.9365</v>
-      </c>
-      <c r="P194">
-        <v>-4.73068</v>
+      <c r="O194" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="P194" s="4" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="195" spans="1:16">
       <c r="A195" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B195" t="s">
         <v>240</v>
@@ -11093,16 +11110,16 @@
       <c r="N195" t="s">
         <v>249</v>
       </c>
-      <c r="O195">
-        <v>-33.0221</v>
-      </c>
-      <c r="P195">
-        <v>-4.89154</v>
+      <c r="O195" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="P195" s="4" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="196" spans="1:16">
       <c r="A196" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B196" t="s">
         <v>240</v>
@@ -11143,16 +11160,16 @@
       <c r="N196" t="s">
         <v>249</v>
       </c>
-      <c r="O196">
-        <v>-32.2454</v>
-      </c>
-      <c r="P196">
-        <v>-4.76908</v>
+      <c r="O196" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="P196" s="4" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="197" spans="1:16">
       <c r="A197" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B197" t="s">
         <v>240</v>
@@ -11193,16 +11210,16 @@
       <c r="N197" t="s">
         <v>249</v>
       </c>
-      <c r="O197">
-        <v>-33.3334</v>
-      </c>
-      <c r="P197">
-        <v>-4.9377</v>
+      <c r="O197" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="P197" s="4" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="198" spans="1:16">
       <c r="A198" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B198" t="s">
         <v>240</v>
@@ -11243,16 +11260,16 @@
       <c r="N198" t="s">
         <v>249</v>
       </c>
-      <c r="O198">
-        <v>-34.1599</v>
-      </c>
-      <c r="P198">
-        <v>-5.0601</v>
+      <c r="O198" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="P198" s="4" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="199" spans="1:16">
       <c r="A199" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B199" t="s">
         <v>240</v>
@@ -11293,16 +11310,16 @@
       <c r="N199" t="s">
         <v>249</v>
       </c>
-      <c r="O199" s="3">
-        <v>-35.297</v>
-      </c>
-      <c r="P199">
-        <v>-5.22853</v>
+      <c r="O199" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="P199" s="4" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="200" spans="1:16">
       <c r="A200" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B200" t="s">
         <v>240</v>
@@ -11343,16 +11360,16 @@
       <c r="N200" t="s">
         <v>249</v>
       </c>
-      <c r="O200" s="3">
-        <v>-35.7038</v>
-      </c>
-      <c r="P200">
-        <v>-5.28891</v>
+      <c r="O200" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="P200" s="4" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="201" spans="1:16">
       <c r="A201" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B201" t="s">
         <v>240</v>
@@ -11393,16 +11410,16 @@
       <c r="N201" t="s">
         <v>249</v>
       </c>
-      <c r="O201" s="3">
-        <v>-36.8485</v>
-      </c>
-      <c r="P201">
-        <v>-5.45838</v>
+      <c r="O201" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="P201" s="4" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="202" spans="1:16">
       <c r="A202" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B202" t="s">
         <v>240</v>
@@ -11443,16 +11460,16 @@
       <c r="N202" t="s">
         <v>249</v>
       </c>
-      <c r="O202" s="3">
-        <v>-37.8228</v>
-      </c>
-      <c r="P202">
-        <v>-5.60281</v>
+      <c r="O202" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="P202" s="4" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="203" spans="1:16">
       <c r="A203" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B203" t="s">
         <v>240</v>
@@ -11493,11 +11510,11 @@
       <c r="N203" t="s">
         <v>249</v>
       </c>
-      <c r="O203" s="3">
-        <v>-38.7088</v>
-      </c>
-      <c r="P203">
-        <v>-5.73398</v>
+      <c r="O203" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="P203" s="4" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="204" spans="1:16" s="1" customFormat="1">
@@ -11552,29 +11569,29 @@
     </row>
     <row r="205" spans="1:16" s="1" customFormat="1">
       <c r="N205" s="1" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="O205" s="3">
-        <v>-64.8019</v>
+        <v>-47.4959</v>
       </c>
       <c r="P205" s="1">
-        <v>-7.85459</v>
+        <v>-5.7569</v>
       </c>
     </row>
     <row r="206" spans="1:16" s="1" customFormat="1">
       <c r="N206" s="1" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="O206" s="2">
-        <v>64.79049999999999</v>
+        <v>48.4135</v>
       </c>
       <c r="P206" s="1">
-        <v>7.85358</v>
+        <v>5.86849</v>
       </c>
     </row>
     <row r="207" spans="1:16" s="1" customFormat="1">
       <c r="N207" s="1" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="O207" s="1">
         <v>35</v>
@@ -11582,7 +11599,7 @@
     </row>
     <row r="208" spans="1:16" s="1" customFormat="1">
       <c r="N208" s="1" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="O208" s="1">
         <v>-35</v>
@@ -11590,7 +11607,7 @@
     </row>
     <row r="209" spans="14:16" s="1" customFormat="1">
       <c r="N209" s="1" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="O209" s="1">
         <v>35</v>
@@ -11598,7 +11615,7 @@
     </row>
     <row r="210" spans="14:16" s="1" customFormat="1">
       <c r="N210" s="1" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="O210" s="1">
         <v>-35</v>
@@ -11606,35 +11623,35 @@
     </row>
     <row r="211" spans="14:16" s="1" customFormat="1">
       <c r="N211" s="1" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="O211" s="1">
-        <v>0.9830637</v>
+        <v>2.198907</v>
       </c>
       <c r="P211" s="1">
-        <v>0.121786</v>
+        <v>0.3062903</v>
       </c>
     </row>
     <row r="212" spans="14:16" s="1" customFormat="1">
       <c r="N212" s="1" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="O212" s="1">
-        <v>34.185427</v>
+        <v>24.473331</v>
       </c>
       <c r="P212" s="1">
-        <v>4.447704</v>
+        <v>3.155384</v>
       </c>
     </row>
     <row r="213" spans="14:16" s="1" customFormat="1">
       <c r="N213" s="1" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="O213" s="1">
-        <v>3477.437627</v>
+        <v>1112.977084</v>
       </c>
       <c r="P213" s="1">
-        <v>3652.065098</v>
+        <v>1030.193904</v>
       </c>
     </row>
     <row r="214" spans="14:16" s="1" customFormat="1"/>

</xml_diff>